<commit_message>
updated to correctly minimize with log likelihood
</commit_message>
<xml_diff>
--- a/wgbs_primary_analysis/sample_key.xlsx
+++ b/wgbs_primary_analysis/sample_key.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Christa.Caggiano/Documents/UCSF_year1/Zaitlen-rotation1/Zaitlen_lab/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Christa.Caggiano/Documents/UCSF_year1/Zaitlen-rotation1/Zaitlen_lab/wgbs_primary_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{505197F3-7F56-3849-AA78-FEE5D2165F9F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="12600" windowHeight="15880" tabRatio="500"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="12600" windowHeight="15740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -110,8 +111,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -208,6 +209,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -475,16 +479,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="C15" sqref="C15:C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -504,7 +508,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -527,7 +531,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -550,7 +554,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -573,7 +577,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -596,7 +600,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -616,7 +620,7 @@
         <v>42844</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -636,7 +640,7 @@
         <v>42881</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -656,7 +660,7 @@
         <v>42923</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -676,99 +680,75 @@
         <v>42965</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="C15" s="10"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="C16" s="11"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C17" s="9">
-        <f>2017-1955</f>
-        <v>62</v>
-      </c>
+    <row r="17" spans="3:4">
+      <c r="C17" s="9"/>
       <c r="D17" s="5"/>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C18" s="10">
-        <f>2017-1960</f>
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C19" s="11">
-        <f>2017-1931</f>
-        <v>86</v>
-      </c>
+    <row r="18" spans="3:4">
+      <c r="C18" s="10"/>
+    </row>
+    <row r="19" spans="3:4">
+      <c r="C19" s="11"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C20" s="9">
-        <f>2017-1953</f>
-        <v>64</v>
-      </c>
+    <row r="20" spans="3:4">
+      <c r="C20" s="9"/>
       <c r="D20" s="5"/>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C21" s="9">
-        <f>2017-1956</f>
-        <v>61</v>
-      </c>
+    <row r="21" spans="3:4">
+      <c r="C21" s="9"/>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C22" s="11">
-        <f>2017-1958</f>
-        <v>59</v>
-      </c>
+    <row r="22" spans="3:4">
+      <c r="C22" s="11"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C23" s="9">
-        <f>2017-1934</f>
-        <v>83</v>
-      </c>
+    <row r="23" spans="3:4">
+      <c r="C23" s="9"/>
       <c r="D23" s="5"/>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C24" s="10">
-        <f>2017-1955</f>
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:4">
+      <c r="C24" s="10"/>
+    </row>
+    <row r="25" spans="3:4">
       <c r="C25" s="10"/>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:4">
       <c r="C26" s="10"/>
     </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:4">
       <c r="C27" s="10"/>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:4">
       <c r="C28" s="10"/>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:4">
       <c r="C29" s="10"/>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:4">
       <c r="C30" s="10"/>
     </row>
   </sheetData>

</xml_diff>